<commit_message>
Updated PayNowSuccessfulNoCFCC Bootstrap Test Case and Test Data
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
+++ b/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA29216-2539-4CE7-B0D9-387429B45EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911AE3EA-CAB5-428C-BA62-7E699907F1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" activeTab="3" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
+    <workbookView xWindow="930" yWindow="7185" windowWidth="21300" windowHeight="8910" activeTab="4" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
   </bookViews>
   <sheets>
     <sheet name="NameData" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>udf data 10</t>
+  </si>
+  <si>
+    <t>2409876325</t>
   </si>
 </sst>
 </file>
@@ -677,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4758406-EDCC-4FC2-8D56-4EE6148C26F6}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,6 +736,11 @@
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -968,10 +976,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB6C1EA-3000-4832-B1CD-65BFF5950FD5}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,6 +1026,11 @@
         <v>64</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1025,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9C5CD7-C2F0-4810-9B2B-3E979499F34C}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,6 +1074,27 @@
         <v>66</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1068,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5A1E49-7B99-423D-9566-8E85E2D36AE6}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,6 +1183,11 @@
         <v>76</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added reuseable library ccPaymentEntryBootstrapPage
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
+++ b/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911AE3EA-CAB5-428C-BA62-7E699907F1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180D0241-135E-43DC-A413-445D9E72205D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="7185" windowWidth="21300" windowHeight="8910" activeTab="4" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
+    <workbookView xWindow="32490" yWindow="2220" windowWidth="25710" windowHeight="12690" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
   </bookViews>
   <sheets>
     <sheet name="NameData" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>2409876325</t>
+  </si>
+  <si>
+    <t>CardholderName</t>
+  </si>
+  <si>
+    <t>Bridges Waters</t>
   </si>
 </sst>
 </file>
@@ -680,21 +686,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4758406-EDCC-4FC2-8D56-4EE6148C26F6}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="13.7109375" style="1"/>
-    <col min="4" max="4" width="25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="13.7109375" style="1"/>
+    <col min="4" max="5" width="25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="13.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,10 +714,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -722,7 +731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -730,17 +739,25 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1040,7 +1057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9C5CD7-C2F0-4810-9B2B-3E979499F34C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added selectPaymentMethodBootstrap and paymentConfirmationBootstrap
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
+++ b/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180D0241-135E-43DC-A413-445D9E72205D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32639E0A-8A9A-4388-AABB-DA5570426A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32490" yWindow="2220" windowWidth="25710" windowHeight="12690" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
+    <workbookView xWindow="3765" yWindow="2520" windowWidth="25710" windowHeight="12690" activeTab="5" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
   </bookViews>
   <sheets>
     <sheet name="NameData" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -244,34 +244,16 @@
     <t>2406983214</t>
   </si>
   <si>
-    <t>udf data 1</t>
-  </si>
-  <si>
     <t>udf data 2</t>
   </si>
   <si>
     <t>udf data 3</t>
   </si>
   <si>
-    <t>udf data 4</t>
-  </si>
-  <si>
-    <t>udf data 5</t>
-  </si>
-  <si>
-    <t>udf data 6</t>
-  </si>
-  <si>
     <t>Orange</t>
   </si>
   <si>
     <t>Soccer</t>
-  </si>
-  <si>
-    <t>udf data 9</t>
-  </si>
-  <si>
-    <t>udf data 10</t>
   </si>
   <si>
     <t>2409876325</t>
@@ -688,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4758406-EDCC-4FC2-8D56-4EE6148C26F6}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -714,7 +696,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -757,7 +739,7 @@
         <v>55</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1096,7 +1078,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5A1E49-7B99-423D-9566-8E85E2D36AE6}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,35 +1151,17 @@
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added ACH Payment Entry Bootstrap Page Reusable Library
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
+++ b/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T476640\Documents\VPS_Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32639E0A-8A9A-4388-AABB-DA5570426A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F16AD1-B619-4A14-B657-B82778ED62E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2520" windowWidth="25710" windowHeight="12690" activeTab="5" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
   </bookViews>
   <sheets>
     <sheet name="NameData" sheetId="1" r:id="rId1"/>
@@ -20,28 +20,17 @@
     <sheet name="EmailAndPhoneData" sheetId="5" r:id="rId5"/>
     <sheet name="UDFData" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -263,6 +252,15 @@
   </si>
   <si>
     <t>Bridges Waters</t>
+  </si>
+  <si>
+    <t>TypeOfAccount</t>
+  </si>
+  <si>
+    <t>Saving</t>
+  </si>
+  <si>
+    <t>Checking</t>
   </si>
 </sst>
 </file>
@@ -674,15 +672,15 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="13.7109375" style="1"/>
+    <col min="1" max="3" width="13.7265625" style="1"/>
     <col min="4" max="5" width="25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="13.7109375" style="1"/>
+    <col min="6" max="6" width="24.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="13.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,7 +700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -713,7 +711,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -721,7 +719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -729,12 +727,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -758,14 +756,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="25.140625" style="1"/>
-    <col min="3" max="3" width="35.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="25.140625" style="1"/>
+    <col min="1" max="2" width="25.1796875" style="1"/>
+    <col min="3" max="3" width="35.1796875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="25.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -805,7 +803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -825,7 +823,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -845,7 +843,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -865,7 +863,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -885,7 +883,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -913,20 +911,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D64820D-36BC-47E5-8B0C-19AD74EF9BDF}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="19.42578125" style="1"/>
-    <col min="3" max="3" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="19.42578125" style="1"/>
+    <col min="1" max="2" width="19.453125" style="1"/>
+    <col min="3" max="3" width="22.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="19.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -939,8 +937,11 @@
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -953,8 +954,11 @@
       <c r="D2" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -966,6 +970,26 @@
       </c>
       <c r="D3" s="1" t="s">
         <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -981,12 +1005,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="22.7109375" style="1"/>
+    <col min="1" max="16384" width="22.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +1024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1011,7 +1035,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -1025,7 +1049,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1043,15 +1067,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="18.42578125" style="1"/>
+    <col min="1" max="1" width="18.453125" style="1"/>
+    <col min="2" max="2" width="27.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="18.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1073,7 +1097,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -1081,12 +1105,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -1103,16 +1127,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5A1E49-7B99-423D-9566-8E85E2D36AE6}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="16.5703125" style="1"/>
+    <col min="1" max="16384" width="16.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1164,7 +1188,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Added test case for Successfull Payment NoCFCorp
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
+++ b/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T476640\Documents\VPS_Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F16AD1-B619-4A14-B657-B82778ED62E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5114D744-C862-4BD6-B2DC-E2BED63BE77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -257,10 +257,22 @@
     <t>TypeOfAccount</t>
   </si>
   <si>
-    <t>Saving</t>
-  </si>
-  <si>
-    <t>Checking</t>
+    <t>EIN</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Personal Saving</t>
+  </si>
+  <si>
+    <t>Personal Checking</t>
+  </si>
+  <si>
+    <t>Corporate Check</t>
+  </si>
+  <si>
+    <t>999999999</t>
   </si>
 </sst>
 </file>
@@ -669,7 +681,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -911,10 +923,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D64820D-36BC-47E5-8B0C-19AD74EF9BDF}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -924,7 +936,7 @@
     <col min="4" max="16384" width="19.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -940,8 +952,14 @@
       <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -955,10 +973,13 @@
         <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -972,10 +993,13 @@
         <v>56</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -988,8 +1012,11 @@
       <c r="D4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>76</v>
+      <c r="F4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1128,7 +1155,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added test cases for successfull payment for Single and dual CF
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
+++ b/KatalonData/IWPBootstrapData/NormalizedSharedData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T476640\Documents\VPS_Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5114D744-C862-4BD6-B2DC-E2BED63BE77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1C57A7-7AD2-4359-B672-65423789A3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BCCB990F-B3AB-4CDA-A16C-818C7712AEED}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -923,10 +923,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D64820D-36BC-47E5-8B0C-19AD74EF9BDF}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1017,6 +1017,23 @@
       </c>
       <c r="G4" s="1" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>